<commit_message>
* Added support for mental ray Arch & Design material. Not complete because it does not support ambient maps yet. * Added Options section to GUI to select material and configure it.
</commit_message>
<xml_diff>
--- a/Material Properties.xlsx
+++ b/Material Properties.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Daz Standard Material" sheetId="1" r:id="rId1"/>
     <sheet name="Max Standard Material" sheetId="2" r:id="rId2"/>
+    <sheet name="mr Arch &amp; Design" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="489">
   <si>
     <t>GlossinessValueMap</t>
   </si>
@@ -708,6 +709,780 @@
   </si>
   <si>
     <t>Diffuse Colour is multiplied with Diffuse Map (if present) and Diffuse Strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  diff_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Diffuse) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fRGBA color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  diff_rough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Diffuse_Roughness) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  diff_weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Diffuse_Weight) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Color) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_gloss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Glossiness) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Samples) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_interp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Interpolation) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_hlonly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Highlights_Only) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Metallic_Reflections) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflectivity) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Color) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_gloss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Glossiness) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Samples) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_interp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Interpolation) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_ior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_IOR) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Transparency) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_trans_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Translucency_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_transc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Translucency_Color) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_transw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Translulcency_Weight) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  anisotropy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  anisoangle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Anisotropy_Angle) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  aniso_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Anisotropy_Mode) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  aniso_channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Anisotropy_Channel) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_func_fresnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Angular_Function_Fresnel) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_func_low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Angular_Function_Low) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_func_high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Angular_Function_High) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_func_curve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Angular_Function_Curve) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_falloff_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Max_Dist_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_falloff_dist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Max_Dist) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_falloff_color_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Max_Dist_Color_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_falloff_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Max_Dist_Color) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_refl_depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Max_Depth) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_cutoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Cutoff_Threshold) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_falloff_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Max_Dist_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_falloff_dist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Max_Dist) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_falloff_color_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Max_Dist_Color_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_falloff_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Max_Dist_Color) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_refr_depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Max_Depth) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_cutoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Cutoff_Threshold) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_indirect_multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Indirect_Multiplier) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_fg_quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(FG_Quality) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  inter_density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Interpolation_Density) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  intr_refl_samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection__Interpolation_points_to_look_up) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  intr_refl_ddist_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Use_detail_distance) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  intr_refl_ddist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Detail_distance) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  intr_refr_samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction__Interpolation_points_to_look_up) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  single_env_sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Single_Environment_Sample) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_round_corners_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Round_Corners_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_round_corners_radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Round_Corners_Radius) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_round_corners_any_mtl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Fillet_against_Any_Material) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_ao_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Enabled) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_ao_exact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_picks_up_colors_from_other_materials__Exact_AO) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_ao_use_global_ambient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Use_Global_Ambient_Light) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_ao_samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Samples) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_ao_distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Distance) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_ao_dark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Shadow_Color) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_ao_ambient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Ambient_Light_Color) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_ao_do_details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_for_GI_FG_detail_enhancement) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_no_area_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Supress_Highlights_for_visible_area_lights) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_1sided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Single_sided_glass___translucency) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_do_refractive_caustics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Do_refractive_caustics) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_skip_inside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Skip_internal_reflections_in_glass__except_TIR) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_hl_to_refl_balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Highlight_vs__Reflection_Balance) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_backface_cull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Back_Face_Culling) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  opts_propagate_alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Propagate_Alpha) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_color_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination_Color_Mode) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_int_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination_Intensity_Mode) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_color_filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_color_kelvin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination_Color_Kelvin) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_int_physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination_Physical_Intensity) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_int_arbitrary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination_Arbitrary_Intensity) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_in_reflections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination___visible_in_Reflections) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_in_fg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination___visible_to_FG) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  no_diffuse_bump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(No_bumps_on_diffuse_shading) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  diff_color_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Diffuse_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  diff_rough_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Roughness_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_color_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_gloss_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Glossiness_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_color_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_gloss_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Glossiness_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_ior_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(IOR_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_transc_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Translucency_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_transw_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Translucency_Weight_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  anisotropy_map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  anisoangle_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Anisotropy_Angle_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_falloff_color_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Fade_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_falloff_color_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Fade_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  indirect_multiplier_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(FG_Multiplier_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  fg_quality_map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ao_dark_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Shadow_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ao_ambient_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Ambient_Light_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  bump_map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  displacement_map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  cutout_map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  environment_map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  add_color_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Additional_Color_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  radius_map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Self_Illumination_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  diff_color_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Diffuse_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  diff_rough_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Roughness_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_color_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_gloss_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Glossiness_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_color_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_gloss_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Glossiness_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_ior_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(IOR_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_transc_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Translucency_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_transw_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Translucency_Weight_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  anisotropy_map_on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  anisoangle_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Anisotropy_Angle_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refl_falloff_color_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reflection_Fade_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  refr_falloff_color_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Refraction_Fade_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  indirect_multiplier_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(FG_Multiplier_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  fg_quality_map_on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ao_dark_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Shadow_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ao_ambient_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AO_Ambient_Light_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  bump_map_on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  displacement_map_on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  cutout_map_on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  environment_map_on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  add_color_map_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Additional_Color_Map_On) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  radius_map_on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  self_illum_map_on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  fg_quality_map_amt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(FG_Quality_Map_Amount) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  bump_map_amt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Bump_Map_Amount) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  displacement_map_amt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Displacement_Map_Amount) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Anisotropy_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(FG_Quality_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Radius_Map) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  mapM23</t>
   </si>
 </sst>
 </file>
@@ -803,7 +1578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -816,6 +1591,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1119,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2542,4 +3318,1587 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D146"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="12" t="s">
+        <v>403</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="12" t="s">
+        <v>405</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="B106" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="B109" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B110" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B111" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="B112" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="C112" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="B114" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="C117" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="B120" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="B121" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="B122" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="C122" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="B123" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="B124" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="B125" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="C125" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="B127" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="C127" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="B128" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="B129" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C129" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="C130" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="B131" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="C131" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="B132" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="C132" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="B133" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="B134" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="B137" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="B138" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="B139" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="B140" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="B141" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="B143" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="C143" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="B144" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="B145" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="C145" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="B146" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="C146" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>